<commit_message>
changed to district aggregate
</commit_message>
<xml_diff>
--- a/TCJA_Localized_Impact.xlsx
+++ b/TCJA_Localized_Impact.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Change to income tax in 2024 if without TCJA ($)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Change to after-tax income in 2024 if without TCJA (%)</t>
+          <t>Change to total individual income tax burden ($ million)</t>
         </is>
       </c>
     </row>
@@ -457,12 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>676</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>-1.83</t>
-        </is>
+        <v>466</v>
       </c>
     </row>
     <row r="3">
@@ -472,12 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>639</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-1.77</t>
-        </is>
+        <v>636</v>
       </c>
     </row>
     <row r="4">
@@ -487,12 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>610</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-1.66</t>
-        </is>
+        <v>669</v>
       </c>
     </row>
     <row r="5">
@@ -502,12 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>561</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-1.62</t>
-        </is>
+        <v>543</v>
       </c>
     </row>
     <row r="6">
@@ -517,12 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>507</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>-1.56</t>
-        </is>
+        <v>326</v>
       </c>
     </row>
     <row r="7">
@@ -532,12 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>552</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-1.64</t>
-        </is>
+        <v>708</v>
       </c>
     </row>
     <row r="8">
@@ -547,12 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>698</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>-1.88</t>
-        </is>
+        <v>524</v>
       </c>
     </row>
     <row r="9">
@@ -562,12 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>497</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>-1.54</t>
-        </is>
+        <v>363</v>
       </c>
     </row>
     <row r="10">
@@ -577,12 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>636</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>-1.79</t>
-        </is>
+        <v>607</v>
       </c>
     </row>
     <row r="11">
@@ -592,12 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>628</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>-1.72</t>
-        </is>
+        <v>253</v>
       </c>
     </row>
     <row r="12">
@@ -607,12 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>575</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>-1.69</t>
-        </is>
+        <v>2105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>